<commit_message>
Adicionando tarefas no backlog da sprint
</commit_message>
<xml_diff>
--- a/Documentação/SprintBacklog.xlsx
+++ b/Documentação/SprintBacklog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Facul BandTec\PI\Projeto PI\blind-market\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\blind-market\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="52">
   <si>
     <t>Requisito</t>
   </si>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t>Pedro</t>
+  </si>
+  <si>
+    <t>Fluxograma do Processo de Atendimento do Suporte</t>
+  </si>
+  <si>
+    <t>Ferramenta de Help Desk configurada e integrada à solução</t>
   </si>
 </sst>
 </file>
@@ -210,7 +216,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -271,6 +277,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -327,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -365,6 +377,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -900,7 +915,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,10 +1361,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,12 +1410,12 @@
         <v>1</v>
       </c>
       <c r="F2" s="13">
-        <f>SUM(B2:B11)</f>
-        <v>144</v>
+        <f>SUM(B2:B19)</f>
+        <v>173</v>
       </c>
       <c r="G2" s="14">
-        <f>SUMIF(D2:D11,0,B2:B11)</f>
-        <v>110</v>
+        <f>SUMIF(D2:D19,0,B2:B19)</f>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1445,7 +1460,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="20" t="s">
         <v>48</v>
@@ -1479,7 +1494,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>48</v>
@@ -1551,6 +1566,34 @@
       </c>
       <c r="E11" s="20" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="17">
+        <v>8</v>
+      </c>
+      <c r="C12" s="21">
+        <v>11</v>
+      </c>
+      <c r="D12" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="17">
+        <v>21</v>
+      </c>
+      <c r="C13" s="21">
+        <v>12</v>
+      </c>
+      <c r="D13" s="18">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1559,18 +1602,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1777,18 +1820,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB45A76C-367E-48F2-BA42-D8633D20F2C2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E79708DC-A660-4460-A0A8-6D647472B58B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E79708DC-A660-4460-A0A8-6D647472B58B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CB45A76C-367E-48F2-BA42-D8633D20F2C2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>